<commit_message>
Working with individual meeting. Fixed some errors. Update databse. Some minor updates for all panels.
</commit_message>
<xml_diff>
--- a/database/mentor_database.xlsx
+++ b/database/mentor_database.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\php_tutorial\minor_project\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F02FB818-CC73-4061-842C-47258886CAB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADBA7704-0EC2-4B70-91BE-E9918DEEB025}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{1890C7C0-D2F1-41DF-AAE6-27CBBCB25E4B}"/>
   </bookViews>
@@ -33,38 +33,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>saratsahariah@gmail.com</t>
   </si>
   <si>
-    <t>Sarat</t>
-  </si>
-  <si>
-    <t>Sahariah</t>
-  </si>
-  <si>
     <t>Computer Science &amp; Engineering</t>
   </si>
   <si>
     <t>nabajyotimedhi@gmail.com</t>
   </si>
   <si>
-    <t>Nabajyoti</t>
-  </si>
-  <si>
     <t>Medhi</t>
   </si>
   <si>
-    <t>rcbmail@gmail.com</t>
-  </si>
-  <si>
-    <t>Ramcharan</t>
-  </si>
-  <si>
-    <t>Bashya</t>
-  </si>
-  <si>
     <t>CSE01</t>
   </si>
   <si>
@@ -72,6 +54,51 @@
   </si>
   <si>
     <t>CSE03</t>
+  </si>
+  <si>
+    <t>Dr. Sarat</t>
+  </si>
+  <si>
+    <t>Saharia</t>
+  </si>
+  <si>
+    <t>Dr. Nabajyoti</t>
+  </si>
+  <si>
+    <t>Pradhan</t>
+  </si>
+  <si>
+    <t>tribikrampradhan@gmail.com</t>
+  </si>
+  <si>
+    <t>CSE04</t>
+  </si>
+  <si>
+    <t>rosysharma@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dr. Rosy </t>
+  </si>
+  <si>
+    <t>Sarmah</t>
+  </si>
+  <si>
+    <t>ECE01</t>
+  </si>
+  <si>
+    <t>Dr. Asim</t>
+  </si>
+  <si>
+    <t>Datta</t>
+  </si>
+  <si>
+    <t>Electrical Engineering</t>
+  </si>
+  <si>
+    <t>asimdatta@gmail.com</t>
+  </si>
+  <si>
+    <t>Dr. Tribikram</t>
   </si>
 </sst>
 </file>
@@ -434,79 +461,119 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FF7205B-F3DA-4163-9ECE-1596C8458A12}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="27.453125" customWidth="1"/>
     <col min="3" max="3" width="15.08984375" customWidth="1"/>
-    <col min="4" max="4" width="11.1796875" customWidth="1"/>
-    <col min="5" max="5" width="11.26953125" customWidth="1"/>
+    <col min="4" max="4" width="13.26953125" customWidth="1"/>
+    <col min="5" max="5" width="17.1796875" customWidth="1"/>
     <col min="6" max="6" width="28.90625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1">
-        <v>7634256459</v>
+        <v>6001020913</v>
       </c>
       <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
         <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C2">
-        <v>3457623489</v>
+        <v>6001020912</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3">
+        <v>6001020910</v>
+      </c>
+      <c r="D3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3">
-        <v>3452367890</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" t="s">
-        <v>3</v>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4">
+        <v>6001020911</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5">
+        <v>6001020909</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -514,7 +581,10 @@
     <hyperlink ref="B1" r:id="rId1" xr:uid="{0F41D3B9-B5FB-4A56-98CD-AC61E57AACB8}"/>
     <hyperlink ref="B2" r:id="rId2" xr:uid="{6982664B-3577-4B54-803A-682EF5BD9703}"/>
     <hyperlink ref="B3" r:id="rId3" xr:uid="{DC0866CE-F10B-4272-BFDD-4024386E3AA7}"/>
+    <hyperlink ref="B4" r:id="rId4" xr:uid="{DE8B3F97-3D42-4BFB-AB13-B7E2C9B9ADA6}"/>
+    <hyperlink ref="B5" r:id="rId5" xr:uid="{0661C9AC-D12D-453B-B510-37CC58F215B6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>